<commit_message>
add reset password and add password endpoints
</commit_message>
<xml_diff>
--- a/Identity/Docs/IdentityDiffs.xlsx
+++ b/Identity/Docs/IdentityDiffs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tests\ELC\ELC.Lite\Identity\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9874BB-888F-471D-A9F2-07BDA6901636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834925C2-1DE8-48EE-8927-0C2D01CFE558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{213926D4-8EA9-4871-8530-369BBBF40EFE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="71">
   <si>
     <t>TryTryTry</t>
   </si>
@@ -234,6 +234,21 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Add to TryTryTry</t>
+  </si>
+  <si>
+    <t>Set to upper case Username</t>
+  </si>
+  <si>
+    <t>Set to upper case Email</t>
+  </si>
+  <si>
+    <t>Set to upper case Name</t>
+  </si>
+  <si>
+    <t>Increase size in TryTryTry</t>
   </si>
 </sst>
 </file>
@@ -289,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -349,11 +364,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -363,15 +387,31 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -383,26 +423,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -717,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4BDC44-A321-4FC1-8B66-B2E175FE125E}">
-  <dimension ref="C2:F68"/>
+  <dimension ref="C2:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,513 +756,541 @@
     <col min="4" max="4" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
+    <row r="2" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="2" t="s">
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="5"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="5"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="6"/>
-      <c r="D8" s="9"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="6"/>
-      <c r="D9" s="9"/>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="5"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="6"/>
-      <c r="D10" s="9"/>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" s="6"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="5" t="s">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="5"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="6"/>
-      <c r="D12" s="9"/>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="5"/>
+      <c r="D12" s="7"/>
       <c r="E12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="6"/>
-      <c r="D13" s="9"/>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="5"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="10" t="s">
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18"/>
+      <c r="H15" s="20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="16" t="s">
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F17" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="16" t="s">
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="17" t="s">
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="16" t="s">
+      <c r="F19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C21" s="2" t="s">
+      <c r="F20" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="20"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="11" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="H23" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C25" s="6"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="18" t="s">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C25" s="5"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C26" s="6"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="18" t="s">
+      <c r="H25" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="5"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C27" s="2" t="s">
+      <c r="F26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C30" s="13" t="s">
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="F30" s="11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C31" s="14" t="s">
+      <c r="H30" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E31" s="14" t="s">
+      <c r="D31" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="13" t="s">
+      <c r="F31" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="13" t="s">
+      <c r="D32" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C33" s="10" t="s">
+      <c r="F32" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="9" t="s">
         <v>39</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="9" t="s">
         <v>39</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="6"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="18" t="s">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C37" s="5"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="F37" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="9" t="s">
         <v>39</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C39" s="2" t="s">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F40" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C41" s="13" t="s">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="13" t="s">
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="E42" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="F42" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="2" t="s">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C43" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C45" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D45" s="20" t="s">
+      <c r="D45" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F45" s="19" t="s">
+      <c r="F45" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="H45" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="14" t="s">
+      <c r="D46" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E46" s="4" t="s">
@@ -1245,21 +1300,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="6"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="19" t="s">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C47" s="5"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="19" t="s">
+      <c r="F47" s="13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="H47" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="I47" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D48" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E48" s="4" t="s">
@@ -1269,21 +1330,27 @@
         <v>23</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C49" s="6"/>
-      <c r="D49" s="15"/>
-      <c r="E49" s="19" t="s">
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C49" s="5"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F49" s="19" t="s">
+      <c r="F49" s="13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="H49" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="I49" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C50" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D50" s="9" t="s">
         <v>57</v>
       </c>
       <c r="E50" s="4" t="s">
@@ -1293,11 +1360,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D51" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E51" s="4" t="s">
@@ -1307,11 +1374,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E52" s="4" t="s">
@@ -1321,21 +1388,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="6"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="19" t="s">
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C53" s="5"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F53" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H53" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C54" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E54" s="4" t="s">
@@ -1345,11 +1415,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C55" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="9" t="s">
         <v>57</v>
       </c>
       <c r="E55" s="4" t="s">
@@ -1359,11 +1429,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C56" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D56" s="9" t="s">
         <v>57</v>
       </c>
       <c r="E56" s="4" t="s">
@@ -1373,21 +1443,24 @@
         <v>57</v>
       </c>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="6"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="19" t="s">
+    <row r="57" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C57" s="5"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F57" s="19" t="s">
+      <c r="F57" s="13" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="H57" s="21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C58" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D58" s="9" t="s">
         <v>57</v>
       </c>
       <c r="E58" s="4" t="s">
@@ -1397,11 +1470,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C59" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D59" s="9" t="s">
         <v>58</v>
       </c>
       <c r="E59" s="4" t="s">
@@ -1411,100 +1484,104 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C60" s="19" t="s">
+    <row r="60" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C60" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D60" s="20" t="s">
+      <c r="D60" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="E60" s="6"/>
-      <c r="F60" s="9"/>
-    </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C61" s="19" t="s">
+      <c r="E60" s="5"/>
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C61" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D61" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E61" s="6"/>
-      <c r="F61" s="9"/>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="19" t="s">
+      <c r="D61" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C62" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D62" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E62" s="6"/>
-      <c r="F62" s="9"/>
-    </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C63" s="2" t="s">
+      <c r="D62" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="5"/>
+      <c r="F62" s="7"/>
+    </row>
+    <row r="63" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C63" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+    </row>
+    <row r="64" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C64" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F64" s="7" t="s">
+      <c r="F64" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D65" s="20" t="s">
+      <c r="D65" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E65" s="6"/>
-      <c r="F65" s="9"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="7"/>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="20" t="s">
+      <c r="D66" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E66" s="6"/>
-      <c r="F66" s="9"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="7"/>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C67" s="19" t="s">
+      <c r="C67" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D67" s="20" t="s">
+      <c r="D67" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E67" s="6"/>
-      <c r="F67" s="9"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="7"/>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C68" s="19" t="s">
+      <c r="C68" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="D68" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E68" s="6"/>
-      <c r="F68" s="9"/>
+      <c r="D68" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E68" s="5"/>
+      <c r="F68" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="H15:H20"/>
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="C43:F43"/>
     <mergeCell ref="C63:F63"/>
@@ -1513,9 +1590,6 @@
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C27:F27"/>
     <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="C3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>